<commit_message>
Add filter column Hoc Luc & Hanh kiem
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="99">
   <si>
     <t>STT</t>
   </si>
@@ -216,21 +216,6 @@
     <t>20</t>
   </si>
   <si>
-    <t>Lê Hồ Nguyên Khôi</t>
-  </si>
-  <si>
-    <t>21/09/2006</t>
-  </si>
-  <si>
-    <t>Khá</t>
-  </si>
-  <si>
-    <t>Học sinh tiên tiến</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Biện Trần Hoài Như</t>
   </si>
   <si>
@@ -295,15 +280,6 @@
   </si>
   <si>
     <t>06/08/2006</t>
-  </si>
-  <si>
-    <t>Trảo Lê Hồng Ánh</t>
-  </si>
-  <si>
-    <t>29/10/2006</t>
-  </si>
-  <si>
-    <t>29</t>
   </si>
   <si>
     <t>Đoàn Nhật Hà</t>
@@ -710,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AA16"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1722,10 +1698,10 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>2102030089</v>
+        <v>2102030100</v>
       </c>
       <c r="D14" t="s">
         <v>67</v>
@@ -1737,46 +1713,46 @@
         <v>8.7</v>
       </c>
       <c r="G14">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="H14">
-        <v>6.3</v>
+        <v>9.5</v>
       </c>
       <c r="I14">
-        <v>6.7</v>
+        <v>9.2</v>
       </c>
       <c r="J14">
-        <v>8.7</v>
+        <v>9.5</v>
       </c>
       <c r="K14">
-        <v>7</v>
+        <v>8.2</v>
       </c>
       <c r="L14">
-        <v>6.7</v>
+        <v>9.2</v>
       </c>
       <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14">
         <v>9.2</v>
       </c>
-      <c r="N14">
-        <v>9</v>
-      </c>
       <c r="O14">
-        <v>8.4</v>
+        <v>9.3</v>
       </c>
       <c r="P14">
-        <v>8.5</v>
+        <v>8.8</v>
       </c>
       <c r="Q14" t="s">
         <v>27</v>
       </c>
       <c r="R14">
-        <v>8.8</v>
+        <v>9.2</v>
       </c>
       <c r="S14" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="T14" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="U14" t="s">
         <v>30</v>
@@ -1791,66 +1767,66 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z14" t="s">
         <v>70</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>2102030100</v>
+        <v>2102030072</v>
       </c>
       <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
         <v>72</v>
       </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
       <c r="F15">
-        <v>8.7</v>
+        <v>8.6</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15">
-        <v>9.5</v>
+        <v>8.6</v>
       </c>
       <c r="I15">
         <v>9.2</v>
       </c>
       <c r="J15">
-        <v>9.5</v>
+        <v>8.7</v>
       </c>
       <c r="K15">
-        <v>8.2</v>
+        <v>8</v>
       </c>
       <c r="L15">
+        <v>8.8</v>
+      </c>
+      <c r="M15">
         <v>9.2</v>
       </c>
-      <c r="M15">
-        <v>10</v>
-      </c>
       <c r="N15">
-        <v>9.2</v>
+        <v>8.6</v>
       </c>
       <c r="O15">
-        <v>9.3</v>
+        <v>9.4</v>
       </c>
       <c r="P15">
-        <v>8.8</v>
+        <v>9.1</v>
       </c>
       <c r="Q15" t="s">
         <v>27</v>
       </c>
       <c r="R15">
-        <v>9.2</v>
+        <v>9.6</v>
       </c>
       <c r="S15" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="T15" t="s">
         <v>29</v>
@@ -1871,48 +1847,48 @@
         <v>31</v>
       </c>
       <c r="Z15" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B16">
-        <v>2102030072</v>
+        <v>2102029541</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F16">
         <v>8.6</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>8.7</v>
       </c>
       <c r="H16">
+        <v>9.8</v>
+      </c>
+      <c r="I16">
+        <v>9.5</v>
+      </c>
+      <c r="J16">
+        <v>8.2</v>
+      </c>
+      <c r="K16">
+        <v>8.1</v>
+      </c>
+      <c r="L16">
         <v>8.6</v>
       </c>
-      <c r="I16">
-        <v>9.2</v>
-      </c>
-      <c r="J16">
-        <v>8.7</v>
-      </c>
-      <c r="K16">
-        <v>8</v>
-      </c>
-      <c r="L16">
-        <v>8.8</v>
-      </c>
       <c r="M16">
-        <v>9.2</v>
+        <v>9.1</v>
       </c>
       <c r="N16">
-        <v>8.6</v>
+        <v>8.9</v>
       </c>
       <c r="O16">
         <v>9.4</v>
@@ -1924,10 +1900,10 @@
         <v>27</v>
       </c>
       <c r="R16">
-        <v>9.6</v>
+        <v>9.3</v>
       </c>
       <c r="S16" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="T16" t="s">
         <v>29</v>
@@ -1936,95 +1912,18 @@
         <v>30</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y16" t="s">
         <v>31</v>
       </c>
       <c r="Z16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>33</v>
-      </c>
-      <c r="B17">
-        <v>2102029541</v>
-      </c>
-      <c r="D17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17">
-        <v>8.6</v>
-      </c>
-      <c r="G17">
-        <v>8.7</v>
-      </c>
-      <c r="H17">
-        <v>9.8</v>
-      </c>
-      <c r="I17">
-        <v>9.5</v>
-      </c>
-      <c r="J17">
-        <v>8.2</v>
-      </c>
-      <c r="K17">
-        <v>8.1</v>
-      </c>
-      <c r="L17">
-        <v>8.6</v>
-      </c>
-      <c r="M17">
-        <v>9.1</v>
-      </c>
-      <c r="N17">
-        <v>8.9</v>
-      </c>
-      <c r="O17">
-        <v>9.4</v>
-      </c>
-      <c r="P17">
-        <v>9.1</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>27</v>
-      </c>
-      <c r="R17">
-        <v>9.3</v>
-      </c>
-      <c r="S17" t="s">
-        <v>51</v>
-      </c>
-      <c r="T17" t="s">
-        <v>29</v>
-      </c>
-      <c r="U17" t="s">
-        <v>30</v>
-      </c>
-      <c r="V17">
-        <v>6</v>
-      </c>
-      <c r="W17">
-        <v>6</v>
-      </c>
-      <c r="X17">
-        <v>6</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z17" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2036,7 +1935,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:AA23"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -2207,10 +2106,10 @@
         <v>2102030100</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F3">
         <v>8.7</v>
@@ -2252,7 +2151,7 @@
         <v>9.2</v>
       </c>
       <c r="S3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="T3" t="s">
         <v>29</v>
@@ -2273,7 +2172,7 @@
         <v>31</v>
       </c>
       <c r="Z3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -2361,10 +2260,10 @@
         <v>2102030101</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F5">
         <v>8.2</v>
@@ -2406,7 +2305,7 @@
         <v>9</v>
       </c>
       <c r="S5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="T5" t="s">
         <v>29</v>
@@ -2427,7 +2326,7 @@
         <v>31</v>
       </c>
       <c r="Z5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -2438,10 +2337,10 @@
         <v>2102030084</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F6">
         <v>8.4</v>
@@ -2515,10 +2414,10 @@
         <v>2102030088</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F7">
         <v>8.2</v>
@@ -2592,10 +2491,10 @@
         <v>2102030102</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F8">
         <v>7.5</v>
@@ -2637,7 +2536,7 @@
         <v>9.4</v>
       </c>
       <c r="S8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="T8" t="s">
         <v>29</v>
@@ -2658,7 +2557,7 @@
         <v>31</v>
       </c>
       <c r="Z8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -2669,10 +2568,10 @@
         <v>2102030071</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F9">
         <v>7.6</v>
@@ -2740,49 +2639,49 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>2102030073</v>
+        <v>2102030082</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="F10">
-        <v>7.7</v>
+        <v>8.7</v>
       </c>
       <c r="G10">
-        <v>6.3</v>
+        <v>7.4</v>
       </c>
       <c r="H10">
-        <v>8.4</v>
+        <v>8.3</v>
       </c>
       <c r="I10">
-        <v>9.5</v>
+        <v>8.7</v>
       </c>
       <c r="J10">
         <v>9</v>
       </c>
       <c r="K10">
+        <v>8.5</v>
+      </c>
+      <c r="L10">
+        <v>7.9</v>
+      </c>
+      <c r="M10">
+        <v>8.9</v>
+      </c>
+      <c r="N10">
         <v>8.7</v>
       </c>
-      <c r="L10">
-        <v>8.3</v>
-      </c>
-      <c r="M10">
-        <v>9.5</v>
-      </c>
-      <c r="N10">
-        <v>9.1</v>
-      </c>
       <c r="O10">
-        <v>9.5</v>
+        <v>9.2</v>
       </c>
       <c r="P10">
-        <v>9.3</v>
+        <v>8.9</v>
       </c>
       <c r="Q10" t="s">
         <v>27</v>
@@ -2791,84 +2690,84 @@
         <v>9.3</v>
       </c>
       <c r="S10" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="U10" t="s">
         <v>30</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="Z10" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B11">
-        <v>2102030082</v>
+        <v>2102030091</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="F11">
-        <v>8.7</v>
+        <v>9.3</v>
       </c>
       <c r="G11">
-        <v>7.4</v>
+        <v>8.2</v>
       </c>
       <c r="H11">
-        <v>8.3</v>
+        <v>9</v>
       </c>
       <c r="I11">
-        <v>8.7</v>
+        <v>8.8</v>
       </c>
       <c r="J11">
         <v>9</v>
       </c>
       <c r="K11">
+        <v>7.4</v>
+      </c>
+      <c r="L11">
         <v>8.5</v>
       </c>
-      <c r="L11">
-        <v>7.9</v>
-      </c>
       <c r="M11">
-        <v>8.9</v>
+        <v>9.1</v>
       </c>
       <c r="N11">
-        <v>8.7</v>
+        <v>9</v>
       </c>
       <c r="O11">
-        <v>9.2</v>
+        <v>9.3</v>
       </c>
       <c r="P11">
-        <v>8.9</v>
+        <v>9.6</v>
       </c>
       <c r="Q11" t="s">
         <v>27</v>
       </c>
       <c r="R11">
-        <v>9.3</v>
+        <v>8.8</v>
       </c>
       <c r="S11" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="T11" t="s">
         <v>29</v>
@@ -2877,63 +2776,63 @@
         <v>30</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" t="s">
         <v>31</v>
       </c>
       <c r="Z11" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>2102030091</v>
+        <v>2102030074</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="F12">
-        <v>9.3</v>
+        <v>8.7</v>
       </c>
       <c r="G12">
-        <v>8.2</v>
+        <v>8.5</v>
       </c>
       <c r="H12">
         <v>9</v>
       </c>
       <c r="I12">
+        <v>9.1</v>
+      </c>
+      <c r="J12">
+        <v>8.9</v>
+      </c>
+      <c r="K12">
+        <v>8.3</v>
+      </c>
+      <c r="L12">
         <v>8.8</v>
       </c>
-      <c r="J12">
-        <v>9</v>
-      </c>
-      <c r="K12">
-        <v>7.4</v>
-      </c>
-      <c r="L12">
-        <v>8.5</v>
-      </c>
       <c r="M12">
-        <v>9.1</v>
+        <v>9.5</v>
       </c>
       <c r="N12">
-        <v>9</v>
+        <v>8.8</v>
       </c>
       <c r="O12">
-        <v>9.3</v>
+        <v>9.8</v>
       </c>
       <c r="P12">
         <v>9.6</v>
@@ -2942,10 +2841,10 @@
         <v>27</v>
       </c>
       <c r="R12">
-        <v>8.8</v>
+        <v>9</v>
       </c>
       <c r="S12" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="T12" t="s">
         <v>29</v>
@@ -2966,51 +2865,51 @@
         <v>31</v>
       </c>
       <c r="Z12" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>2102030074</v>
+        <v>2102030077</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F13">
-        <v>8.7</v>
+        <v>7.9</v>
       </c>
       <c r="G13">
-        <v>8.5</v>
+        <v>6.9</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <v>7.9</v>
       </c>
       <c r="I13">
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="J13">
         <v>8.9</v>
       </c>
       <c r="K13">
-        <v>8.3</v>
+        <v>7.9</v>
       </c>
       <c r="L13">
-        <v>8.8</v>
+        <v>8.2</v>
       </c>
       <c r="M13">
-        <v>9.5</v>
+        <v>8.7</v>
       </c>
       <c r="N13">
-        <v>8.8</v>
+        <v>8.6</v>
       </c>
       <c r="O13">
-        <v>9.8</v>
+        <v>8.7</v>
       </c>
       <c r="P13">
         <v>9.6</v>
@@ -3019,10 +2918,10 @@
         <v>27</v>
       </c>
       <c r="R13">
-        <v>9</v>
+        <v>9.4</v>
       </c>
       <c r="S13" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="T13" t="s">
         <v>29</v>
@@ -3031,45 +2930,45 @@
         <v>30</v>
       </c>
       <c r="V13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="s">
         <v>31</v>
       </c>
       <c r="Z13" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>2102030077</v>
+        <v>2102030085</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="F14">
-        <v>7.9</v>
+        <v>9</v>
       </c>
       <c r="G14">
-        <v>6.9</v>
+        <v>8.2</v>
       </c>
       <c r="H14">
-        <v>7.9</v>
+        <v>9</v>
       </c>
       <c r="I14">
-        <v>8.1</v>
+        <v>9.4</v>
       </c>
       <c r="J14">
         <v>8.9</v>
@@ -3078,16 +2977,16 @@
         <v>7.9</v>
       </c>
       <c r="L14">
-        <v>8.2</v>
+        <v>9.3</v>
       </c>
       <c r="M14">
-        <v>8.7</v>
+        <v>9.2</v>
       </c>
       <c r="N14">
-        <v>8.6</v>
+        <v>9</v>
       </c>
       <c r="O14">
-        <v>8.7</v>
+        <v>9.5</v>
       </c>
       <c r="P14">
         <v>9.6</v>
@@ -3096,10 +2995,10 @@
         <v>27</v>
       </c>
       <c r="R14">
-        <v>9.4</v>
+        <v>9.3</v>
       </c>
       <c r="S14" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="T14" t="s">
         <v>29</v>
@@ -3108,75 +3007,75 @@
         <v>30</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" t="s">
         <v>31</v>
       </c>
       <c r="Z14" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>2102030085</v>
+        <v>2102030083</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="F15">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="G15">
-        <v>8.2</v>
+        <v>7.7</v>
       </c>
       <c r="H15">
-        <v>9</v>
+        <v>7.6</v>
       </c>
       <c r="I15">
-        <v>9.4</v>
+        <v>8.8</v>
       </c>
       <c r="J15">
-        <v>8.9</v>
+        <v>8.8</v>
       </c>
       <c r="K15">
         <v>7.9</v>
       </c>
       <c r="L15">
-        <v>9.3</v>
+        <v>8.2</v>
       </c>
       <c r="M15">
+        <v>9</v>
+      </c>
+      <c r="N15">
         <v>9.2</v>
       </c>
-      <c r="N15">
-        <v>9</v>
-      </c>
       <c r="O15">
-        <v>9.5</v>
+        <v>9.4</v>
       </c>
       <c r="P15">
-        <v>9.6</v>
+        <v>7.9</v>
       </c>
       <c r="Q15" t="s">
         <v>27</v>
       </c>
       <c r="R15">
-        <v>9.3</v>
+        <v>9.1</v>
       </c>
       <c r="S15" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="T15" t="s">
         <v>29</v>
@@ -3185,75 +3084,75 @@
         <v>30</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="s">
         <v>31</v>
       </c>
       <c r="Z15" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <v>2102030083</v>
+        <v>2102030097</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F16">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="G16">
-        <v>7.7</v>
+        <v>7.9</v>
       </c>
       <c r="H16">
-        <v>7.6</v>
+        <v>8.5</v>
       </c>
       <c r="I16">
-        <v>8.8</v>
+        <v>8</v>
       </c>
       <c r="J16">
         <v>8.8</v>
       </c>
       <c r="K16">
-        <v>7.9</v>
+        <v>8.2</v>
       </c>
       <c r="L16">
         <v>8.2</v>
       </c>
       <c r="M16">
-        <v>9</v>
+        <v>9.3</v>
       </c>
       <c r="N16">
-        <v>9.2</v>
+        <v>8.7</v>
       </c>
       <c r="O16">
-        <v>9.4</v>
+        <v>9.3</v>
       </c>
       <c r="P16">
-        <v>7.9</v>
+        <v>9.6</v>
       </c>
       <c r="Q16" t="s">
         <v>27</v>
       </c>
       <c r="R16">
-        <v>9.1</v>
+        <v>9.2</v>
       </c>
       <c r="S16" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="T16" t="s">
         <v>29</v>
@@ -3274,60 +3173,60 @@
         <v>31</v>
       </c>
       <c r="Z16" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>2102030097</v>
+        <v>2102030072</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="F17">
-        <v>8.1</v>
+        <v>8.6</v>
       </c>
       <c r="G17">
-        <v>7.9</v>
+        <v>7</v>
       </c>
       <c r="H17">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="I17">
+        <v>9.2</v>
+      </c>
+      <c r="J17">
+        <v>8.7</v>
+      </c>
+      <c r="K17">
         <v>8</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>8.8</v>
       </c>
-      <c r="K17">
-        <v>8.2</v>
-      </c>
-      <c r="L17">
-        <v>8.2</v>
-      </c>
       <c r="M17">
-        <v>9.3</v>
+        <v>9.2</v>
       </c>
       <c r="N17">
-        <v>8.7</v>
+        <v>8.6</v>
       </c>
       <c r="O17">
-        <v>9.3</v>
+        <v>9.4</v>
       </c>
       <c r="P17">
-        <v>9.6</v>
+        <v>9.1</v>
       </c>
       <c r="Q17" t="s">
         <v>27</v>
       </c>
       <c r="R17">
-        <v>9.2</v>
+        <v>9.6</v>
       </c>
       <c r="S17" t="s">
         <v>35</v>
@@ -3356,58 +3255,58 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>2102030072</v>
+        <v>2102030075</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F18">
+        <v>8.7</v>
+      </c>
+      <c r="G18">
+        <v>8.8</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
         <v>8.6</v>
-      </c>
-      <c r="G18">
-        <v>7</v>
-      </c>
-      <c r="H18">
-        <v>8.6</v>
-      </c>
-      <c r="I18">
-        <v>9.2</v>
       </c>
       <c r="J18">
         <v>8.7</v>
       </c>
       <c r="K18">
-        <v>8</v>
+        <v>7.9</v>
       </c>
       <c r="L18">
-        <v>8.8</v>
+        <v>8.7</v>
       </c>
       <c r="M18">
-        <v>9.2</v>
+        <v>9.5</v>
       </c>
       <c r="N18">
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
       <c r="O18">
-        <v>9.4</v>
+        <v>9.7</v>
       </c>
       <c r="P18">
-        <v>9.1</v>
+        <v>8.9</v>
       </c>
       <c r="Q18" t="s">
         <v>27</v>
       </c>
       <c r="R18">
-        <v>9.6</v>
+        <v>9.4</v>
       </c>
       <c r="S18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="T18" t="s">
         <v>29</v>
@@ -3428,63 +3327,63 @@
         <v>31</v>
       </c>
       <c r="Z18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>2102030075</v>
+        <v>2102030076</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="F19">
-        <v>8.7</v>
+        <v>8.3</v>
       </c>
       <c r="G19">
-        <v>8.8</v>
+        <v>7.5</v>
       </c>
       <c r="H19">
-        <v>8</v>
+        <v>6.6</v>
       </c>
       <c r="I19">
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
       <c r="J19">
         <v>8.7</v>
       </c>
       <c r="K19">
-        <v>7.9</v>
+        <v>8.7</v>
       </c>
       <c r="L19">
         <v>8.7</v>
       </c>
       <c r="M19">
+        <v>9.3</v>
+      </c>
+      <c r="N19">
+        <v>9.3</v>
+      </c>
+      <c r="O19">
         <v>9.5</v>
       </c>
-      <c r="N19">
-        <v>9.1</v>
-      </c>
-      <c r="O19">
-        <v>9.7</v>
-      </c>
       <c r="P19">
-        <v>8.9</v>
+        <v>9.6</v>
       </c>
       <c r="Q19" t="s">
         <v>27</v>
       </c>
       <c r="R19">
-        <v>9.4</v>
+        <v>9.2</v>
       </c>
       <c r="S19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="T19" t="s">
         <v>29</v>
@@ -3493,75 +3392,75 @@
         <v>30</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" t="s">
         <v>31</v>
       </c>
       <c r="Z19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>2102030076</v>
+        <v>2102030099</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F20">
-        <v>8.3</v>
+        <v>8.2</v>
       </c>
       <c r="G20">
-        <v>7.5</v>
+        <v>7.8</v>
       </c>
       <c r="H20">
-        <v>6.6</v>
+        <v>8.2</v>
       </c>
       <c r="I20">
-        <v>9.1</v>
+        <v>9.4</v>
       </c>
       <c r="J20">
         <v>8.7</v>
       </c>
       <c r="K20">
-        <v>8.7</v>
+        <v>8.1</v>
       </c>
       <c r="L20">
         <v>8.7</v>
       </c>
       <c r="M20">
-        <v>9.3</v>
+        <v>9.8</v>
       </c>
       <c r="N20">
         <v>9.3</v>
       </c>
       <c r="O20">
-        <v>9.5</v>
+        <v>8.8</v>
       </c>
       <c r="P20">
-        <v>9.6</v>
+        <v>9.4</v>
       </c>
       <c r="Q20" t="s">
         <v>27</v>
       </c>
       <c r="R20">
-        <v>9.2</v>
+        <v>9</v>
       </c>
       <c r="S20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="T20" t="s">
         <v>29</v>
@@ -3582,140 +3481,140 @@
         <v>31</v>
       </c>
       <c r="Z20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>2102030089</v>
+        <v>2102030078</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="F21">
-        <v>8.7</v>
+        <v>9.2</v>
       </c>
       <c r="G21">
-        <v>7.7</v>
+        <v>7.8</v>
       </c>
       <c r="H21">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I21">
-        <v>6.7</v>
+        <v>9.3</v>
       </c>
       <c r="J21">
-        <v>8.7</v>
+        <v>8.6</v>
       </c>
       <c r="K21">
-        <v>7</v>
+        <v>8.4</v>
       </c>
       <c r="L21">
-        <v>6.7</v>
+        <v>8.4</v>
       </c>
       <c r="M21">
+        <v>9.3</v>
+      </c>
+      <c r="N21">
+        <v>9.1</v>
+      </c>
+      <c r="O21">
+        <v>8.8</v>
+      </c>
+      <c r="P21">
         <v>9.2</v>
-      </c>
-      <c r="N21">
-        <v>9</v>
-      </c>
-      <c r="O21">
-        <v>8.4</v>
-      </c>
-      <c r="P21">
-        <v>8.5</v>
       </c>
       <c r="Q21" t="s">
         <v>27</v>
       </c>
       <c r="R21">
-        <v>8.8</v>
+        <v>9.2</v>
       </c>
       <c r="S21" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="T21" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="U21" t="s">
         <v>30</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y21" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="Z21" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B22">
-        <v>2102030099</v>
+        <v>2102030086</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>34</v>
       </c>
       <c r="F22">
+        <v>9.3</v>
+      </c>
+      <c r="G22">
         <v>8.2</v>
       </c>
-      <c r="G22">
-        <v>7.8</v>
-      </c>
       <c r="H22">
-        <v>8.2</v>
+        <v>9.4</v>
       </c>
       <c r="I22">
-        <v>9.4</v>
+        <v>8.1</v>
       </c>
       <c r="J22">
-        <v>8.7</v>
+        <v>8.6</v>
       </c>
       <c r="K22">
-        <v>8.1</v>
+        <v>7.9</v>
       </c>
       <c r="L22">
-        <v>8.7</v>
+        <v>8.3</v>
       </c>
       <c r="M22">
-        <v>9.8</v>
+        <v>8.8</v>
       </c>
       <c r="N22">
         <v>9.3</v>
       </c>
       <c r="O22">
-        <v>8.8</v>
+        <v>8.4</v>
       </c>
       <c r="P22">
-        <v>9.4</v>
+        <v>8.9</v>
       </c>
       <c r="Q22" t="s">
         <v>27</v>
       </c>
       <c r="R22">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="S22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="T22" t="s">
         <v>29</v>
@@ -3736,30 +3635,30 @@
         <v>31</v>
       </c>
       <c r="Z22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B23">
-        <v>2102030078</v>
+        <v>2102030103</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F23">
-        <v>9.2</v>
+        <v>8.9</v>
       </c>
       <c r="G23">
-        <v>7.8</v>
+        <v>7.4</v>
       </c>
       <c r="H23">
-        <v>7.9</v>
+        <v>8.6</v>
       </c>
       <c r="I23">
         <v>9.3</v>
@@ -3768,31 +3667,31 @@
         <v>8.6</v>
       </c>
       <c r="K23">
-        <v>8.4</v>
+        <v>8.6</v>
       </c>
       <c r="L23">
-        <v>8.4</v>
+        <v>8</v>
       </c>
       <c r="M23">
-        <v>9.3</v>
+        <v>8.9</v>
       </c>
       <c r="N23">
         <v>9.1</v>
       </c>
       <c r="O23">
-        <v>8.8</v>
+        <v>9.2</v>
       </c>
       <c r="P23">
-        <v>9.2</v>
+        <v>9.1</v>
       </c>
       <c r="Q23" t="s">
         <v>27</v>
       </c>
       <c r="R23">
-        <v>9.2</v>
+        <v>9.1</v>
       </c>
       <c r="S23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="T23" t="s">
         <v>29</v>
@@ -3813,160 +3712,6 @@
         <v>31</v>
       </c>
       <c r="Z23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>15</v>
-      </c>
-      <c r="B24">
-        <v>2102030086</v>
-      </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24">
-        <v>9.3</v>
-      </c>
-      <c r="G24">
-        <v>8.2</v>
-      </c>
-      <c r="H24">
-        <v>9.4</v>
-      </c>
-      <c r="I24">
-        <v>8.1</v>
-      </c>
-      <c r="J24">
-        <v>8.6</v>
-      </c>
-      <c r="K24">
-        <v>7.9</v>
-      </c>
-      <c r="L24">
-        <v>8.3</v>
-      </c>
-      <c r="M24">
-        <v>8.8</v>
-      </c>
-      <c r="N24">
-        <v>9.3</v>
-      </c>
-      <c r="O24">
-        <v>8.4</v>
-      </c>
-      <c r="P24">
-        <v>8.9</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>27</v>
-      </c>
-      <c r="R24">
-        <v>9.5</v>
-      </c>
-      <c r="S24" t="s">
-        <v>35</v>
-      </c>
-      <c r="T24" t="s">
-        <v>29</v>
-      </c>
-      <c r="U24" t="s">
-        <v>30</v>
-      </c>
-      <c r="V24">
-        <v>1</v>
-      </c>
-      <c r="W24">
-        <v>1</v>
-      </c>
-      <c r="X24">
-        <v>1</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>29</v>
-      </c>
-      <c r="B25">
-        <v>2102030103</v>
-      </c>
-      <c r="D25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25">
-        <v>8.9</v>
-      </c>
-      <c r="G25">
-        <v>7.4</v>
-      </c>
-      <c r="H25">
-        <v>8.6</v>
-      </c>
-      <c r="I25">
-        <v>9.3</v>
-      </c>
-      <c r="J25">
-        <v>8.6</v>
-      </c>
-      <c r="K25">
-        <v>8.6</v>
-      </c>
-      <c r="L25">
-        <v>8</v>
-      </c>
-      <c r="M25">
-        <v>8.9</v>
-      </c>
-      <c r="N25">
-        <v>9.1</v>
-      </c>
-      <c r="O25">
-        <v>9.2</v>
-      </c>
-      <c r="P25">
-        <v>9.1</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>27</v>
-      </c>
-      <c r="R25">
-        <v>9.1</v>
-      </c>
-      <c r="S25" t="s">
-        <v>35</v>
-      </c>
-      <c r="T25" t="s">
-        <v>29</v>
-      </c>
-      <c r="U25" t="s">
-        <v>30</v>
-      </c>
-      <c r="V25">
-        <v>3</v>
-      </c>
-      <c r="W25">
-        <v>3</v>
-      </c>
-      <c r="X25">
-        <v>3</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z25" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4303,10 +4048,10 @@
         <v>2102029541</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F5">
         <v>8.6</v>

</xml_diff>